<commit_message>
Marked a few strings for translation.
</commit_message>
<xml_diff>
--- a/tools/i18n/Filelist.xlsx
+++ b/tools/i18n/Filelist.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="664" uniqueCount="612">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="694" uniqueCount="612">
   <si>
     <t>brushmanip.cpp</t>
   </si>
@@ -1918,7 +1918,7 @@
     <cellStyle name="Prozent" xfId="1" builtinId="5"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="14">
+  <dxfs count="9">
     <dxf>
       <font>
         <condense val="0"/>
@@ -1972,66 +1972,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2375,8 +2315,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E621"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1470" topLeftCell="A61" activePane="bottomLeft"/>
+      <selection activeCell="D1" sqref="D1:E4"/>
+      <selection pane="bottomLeft" activeCell="B70" sqref="B70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2405,7 +2347,7 @@
       </c>
       <c r="E2">
         <f>COUNTIF(B2:B621,"ok")</f>
-        <v>39</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -2420,7 +2362,7 @@
       </c>
       <c r="E3">
         <f>COUNTIF(B2:B621,"")</f>
-        <v>581</v>
+        <v>551</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -2435,7 +2377,7 @@
       </c>
       <c r="E4" s="3">
         <f>E2/E3</f>
-        <v>6.7125645438898457E-2</v>
+        <v>0.12522686025408347</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -2730,198 +2672,288 @@
       <c r="A41" t="s">
         <v>506</v>
       </c>
+      <c r="B41" s="1" t="s">
+        <v>603</v>
+      </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" t="s">
         <v>33</v>
       </c>
+      <c r="B42" s="1" t="s">
+        <v>603</v>
+      </c>
     </row>
     <row r="43" spans="1:2">
       <c r="A43" t="s">
         <v>34</v>
       </c>
+      <c r="B43" s="1" t="s">
+        <v>603</v>
+      </c>
     </row>
     <row r="44" spans="1:2">
       <c r="A44" t="s">
         <v>507</v>
       </c>
+      <c r="B44" s="1" t="s">
+        <v>603</v>
+      </c>
     </row>
     <row r="45" spans="1:2">
       <c r="A45" t="s">
         <v>35</v>
       </c>
+      <c r="B45" s="1" t="s">
+        <v>603</v>
+      </c>
     </row>
     <row r="46" spans="1:2">
       <c r="A46" t="s">
         <v>36</v>
       </c>
+      <c r="B46" s="1" t="s">
+        <v>603</v>
+      </c>
     </row>
     <row r="47" spans="1:2">
       <c r="A47" t="s">
         <v>37</v>
       </c>
+      <c r="B47" s="1" t="s">
+        <v>603</v>
+      </c>
     </row>
     <row r="48" spans="1:2">
       <c r="A48" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="49" spans="1:1">
+      <c r="B48" s="1" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
       <c r="A49" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="50" spans="1:1">
+      <c r="B49" s="1" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
       <c r="A50" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="51" spans="1:1">
+      <c r="B50" s="1" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
       <c r="A51" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="52" spans="1:1">
+      <c r="B51" s="1" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
       <c r="A52" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="53" spans="1:1">
+      <c r="B52" s="1" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
       <c r="A53" t="s">
         <v>508</v>
       </c>
-    </row>
-    <row r="54" spans="1:1">
+      <c r="B53" s="1" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
       <c r="A54" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="55" spans="1:1">
+      <c r="B54" s="1" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
       <c r="A55" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="56" spans="1:1">
+      <c r="B55" s="1" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
       <c r="A56" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="57" spans="1:1">
+      <c r="B56" s="1" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
       <c r="A57" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="58" spans="1:1">
+      <c r="B57" s="1" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
       <c r="A58" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="59" spans="1:1">
+      <c r="B58" s="1" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
       <c r="A59" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="60" spans="1:1">
+      <c r="B59" s="1" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
       <c r="A60" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="61" spans="1:1">
+      <c r="B60" s="1" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2">
       <c r="A61" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="62" spans="1:1">
+      <c r="B61" s="1" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2">
       <c r="A62" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="63" spans="1:1">
+      <c r="B62" s="1" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2">
       <c r="A63" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="64" spans="1:1">
+      <c r="B63" s="1" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2">
       <c r="A64" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="65" spans="1:1">
+      <c r="B64" s="1" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2">
       <c r="A65" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="66" spans="1:1">
+      <c r="B65" s="1" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2">
       <c r="A66" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="67" spans="1:1">
+      <c r="B66" s="1" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2">
       <c r="A67" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="68" spans="1:1">
+      <c r="B67" s="1" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2">
       <c r="A68" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="69" spans="1:1">
+      <c r="B68" s="1" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2">
       <c r="A69" t="s">
         <v>509</v>
       </c>
-    </row>
-    <row r="70" spans="1:1">
+      <c r="B69" s="1" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2">
       <c r="A70" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="71" spans="1:1">
+      <c r="B70" s="1" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2">
       <c r="A71" t="s">
         <v>510</v>
       </c>
     </row>
-    <row r="72" spans="1:1">
+    <row r="72" spans="1:2">
       <c r="A72" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="73" spans="1:1">
+    <row r="73" spans="1:2">
       <c r="A73" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="74" spans="1:1">
+    <row r="74" spans="1:2">
       <c r="A74" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="75" spans="1:1">
+    <row r="75" spans="1:2">
       <c r="A75" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="76" spans="1:1">
+    <row r="76" spans="1:2">
       <c r="A76" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="77" spans="1:1">
+    <row r="77" spans="1:2">
       <c r="A77" t="s">
         <v>511</v>
       </c>
     </row>
-    <row r="78" spans="1:1">
+    <row r="78" spans="1:2">
       <c r="A78" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="79" spans="1:1">
+    <row r="79" spans="1:2">
       <c r="A79" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="80" spans="1:1">
+    <row r="80" spans="1:2">
       <c r="A80" t="s">
         <v>512</v>
       </c>

</xml_diff>

<commit_message>
Marked a few strings for translation. First pass finished.
</commit_message>
<xml_diff>
--- a/tools/i18n/Filelist.xlsx
+++ b/tools/i18n/Filelist.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1157" uniqueCount="619">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1251" uniqueCount="619">
   <si>
     <t>brushmanip.cpp</t>
   </si>
@@ -1939,7 +1939,139 @@
     <cellStyle name="Prozent" xfId="1" builtinId="5"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="17">
+  <dxfs count="29">
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <condense val="0"/>
@@ -2421,9 +2553,9 @@
   <dimension ref="A1:E621"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <pane ySplit="1470" topLeftCell="A514" activePane="bottomLeft"/>
+      <pane ySplit="1470" topLeftCell="A157" activePane="bottomLeft"/>
       <selection activeCell="E5" sqref="E5"/>
-      <selection pane="bottomLeft" activeCell="B528" sqref="B528"/>
+      <selection pane="bottomLeft" activeCell="A163" sqref="A163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2452,7 +2584,7 @@
       </c>
       <c r="E2">
         <f>COUNTIF(B2:B621,"ok")</f>
-        <v>525</v>
+        <v>619</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -2467,7 +2599,7 @@
       </c>
       <c r="E3">
         <f>COUNTIF(B2:B621,"")</f>
-        <v>95</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -2482,7 +2614,7 @@
       </c>
       <c r="E4" s="3">
         <f>E2/(E2+E3)</f>
-        <v>0.84677419354838712</v>
+        <v>0.99838709677419357</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -4835,6 +4967,9 @@
       <c r="A296" t="s">
         <v>557</v>
       </c>
+      <c r="B296" s="1" t="s">
+        <v>603</v>
+      </c>
     </row>
     <row r="297" spans="1:3">
       <c r="A297" t="s">
@@ -6680,71 +6815,113 @@
       <c r="A527" t="s">
         <v>588</v>
       </c>
+      <c r="B527" s="1" t="s">
+        <v>603</v>
+      </c>
     </row>
     <row r="528" spans="1:2">
       <c r="A528" t="s">
         <v>423</v>
       </c>
+      <c r="B528" s="1" t="s">
+        <v>603</v>
+      </c>
     </row>
     <row r="529" spans="1:2">
       <c r="A529" t="s">
         <v>605</v>
       </c>
+      <c r="B529" s="1" t="s">
+        <v>603</v>
+      </c>
     </row>
     <row r="530" spans="1:2">
       <c r="A530" t="s">
         <v>424</v>
       </c>
+      <c r="B530" s="1" t="s">
+        <v>603</v>
+      </c>
     </row>
     <row r="531" spans="1:2">
       <c r="A531" t="s">
         <v>425</v>
       </c>
+      <c r="B531" s="1" t="s">
+        <v>603</v>
+      </c>
     </row>
     <row r="532" spans="1:2">
       <c r="A532" t="s">
         <v>426</v>
       </c>
+      <c r="B532" s="1" t="s">
+        <v>603</v>
+      </c>
     </row>
     <row r="533" spans="1:2">
       <c r="A533" t="s">
         <v>589</v>
       </c>
+      <c r="B533" s="1" t="s">
+        <v>603</v>
+      </c>
     </row>
     <row r="534" spans="1:2">
       <c r="A534" t="s">
         <v>193</v>
       </c>
+      <c r="B534" s="1" t="s">
+        <v>603</v>
+      </c>
     </row>
     <row r="535" spans="1:2">
       <c r="A535" t="s">
         <v>427</v>
       </c>
+      <c r="B535" s="1" t="s">
+        <v>603</v>
+      </c>
     </row>
     <row r="536" spans="1:2">
       <c r="A536" t="s">
         <v>428</v>
       </c>
+      <c r="B536" s="1" t="s">
+        <v>603</v>
+      </c>
     </row>
     <row r="537" spans="1:2">
       <c r="A537" t="s">
         <v>590</v>
       </c>
+      <c r="B537" s="1" t="s">
+        <v>603</v>
+      </c>
     </row>
     <row r="538" spans="1:2">
       <c r="A538" t="s">
         <v>429</v>
       </c>
+      <c r="B538" s="1" t="s">
+        <v>603</v>
+      </c>
     </row>
     <row r="539" spans="1:2">
       <c r="A539" t="s">
         <v>430</v>
       </c>
+      <c r="B539" s="1" t="s">
+        <v>603</v>
+      </c>
     </row>
     <row r="540" spans="1:2">
       <c r="A540" t="s">
         <v>431</v>
       </c>
+      <c r="B540" s="1" t="s">
+        <v>603</v>
+      </c>
     </row>
     <row r="541" spans="1:2">
       <c r="A541" t="s">
@@ -6766,408 +6943,645 @@
       <c r="A543" t="s">
         <v>592</v>
       </c>
+      <c r="B543" s="1" t="s">
+        <v>603</v>
+      </c>
     </row>
     <row r="544" spans="1:2">
       <c r="A544" t="s">
         <v>433</v>
       </c>
-    </row>
-    <row r="545" spans="1:1">
+      <c r="B544" s="1" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="545" spans="1:2">
       <c r="A545" t="s">
         <v>593</v>
       </c>
-    </row>
-    <row r="546" spans="1:1">
+      <c r="B545" s="1" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="546" spans="1:2">
       <c r="A546" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="547" spans="1:1">
+      <c r="B546" s="1" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="547" spans="1:2">
       <c r="A547" t="s">
         <v>435</v>
       </c>
-    </row>
-    <row r="548" spans="1:1">
+      <c r="B547" s="1" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="548" spans="1:2">
       <c r="A548" t="s">
         <v>436</v>
       </c>
-    </row>
-    <row r="549" spans="1:1">
+      <c r="B548" s="1" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="549" spans="1:2">
       <c r="A549" t="s">
         <v>437</v>
       </c>
-    </row>
-    <row r="550" spans="1:1">
+      <c r="B549" s="1" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="550" spans="1:2">
       <c r="A550" t="s">
         <v>438</v>
       </c>
-    </row>
-    <row r="551" spans="1:1">
+      <c r="B550" s="1" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="551" spans="1:2">
       <c r="A551" t="s">
         <v>439</v>
       </c>
-    </row>
-    <row r="552" spans="1:1">
+      <c r="B551" s="1" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="552" spans="1:2">
       <c r="A552" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="553" spans="1:1">
+      <c r="B552" s="1" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="553" spans="1:2">
       <c r="A553" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="554" spans="1:1">
+      <c r="B553" s="1" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="554" spans="1:2">
       <c r="A554" t="s">
         <v>442</v>
       </c>
-    </row>
-    <row r="555" spans="1:1">
+      <c r="B554" s="1" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="555" spans="1:2">
       <c r="A555" t="s">
         <v>443</v>
       </c>
-    </row>
-    <row r="556" spans="1:1">
+      <c r="B555" s="1" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="556" spans="1:2">
       <c r="A556" t="s">
         <v>444</v>
       </c>
-    </row>
-    <row r="557" spans="1:1">
+      <c r="B556" s="1" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="557" spans="1:2">
       <c r="A557" t="s">
         <v>445</v>
       </c>
-    </row>
-    <row r="558" spans="1:1">
+      <c r="B557" s="1" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="558" spans="1:2">
       <c r="A558" t="s">
         <v>446</v>
       </c>
-    </row>
-    <row r="559" spans="1:1">
+      <c r="B558" s="1" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="559" spans="1:2">
       <c r="A559" t="s">
         <v>447</v>
       </c>
-    </row>
-    <row r="560" spans="1:1">
+      <c r="B559" s="1" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="560" spans="1:2">
       <c r="A560" t="s">
         <v>448</v>
       </c>
-    </row>
-    <row r="561" spans="1:1">
+      <c r="B560" s="1" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="561" spans="1:2">
       <c r="A561" t="s">
         <v>449</v>
       </c>
-    </row>
-    <row r="562" spans="1:1">
+      <c r="B561" s="1" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="562" spans="1:2">
       <c r="A562" t="s">
         <v>450</v>
       </c>
-    </row>
-    <row r="563" spans="1:1">
+      <c r="B562" s="1" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="563" spans="1:2">
       <c r="A563" t="s">
         <v>451</v>
       </c>
-    </row>
-    <row r="564" spans="1:1">
+      <c r="B563" s="1" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="564" spans="1:2">
       <c r="A564" t="s">
         <v>452</v>
       </c>
-    </row>
-    <row r="565" spans="1:1">
+      <c r="B564" s="1" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="565" spans="1:2">
       <c r="A565" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="566" spans="1:1">
+      <c r="B565" s="1" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="566" spans="1:2">
       <c r="A566" t="s">
         <v>454</v>
       </c>
-    </row>
-    <row r="567" spans="1:1">
+      <c r="B566" s="1" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="567" spans="1:2">
       <c r="A567" t="s">
         <v>594</v>
       </c>
-    </row>
-    <row r="568" spans="1:1">
+      <c r="B567" s="1" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="568" spans="1:2">
       <c r="A568" t="s">
         <v>455</v>
       </c>
-    </row>
-    <row r="569" spans="1:1">
+      <c r="B568" s="1" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="569" spans="1:2">
       <c r="A569" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="570" spans="1:1">
+      <c r="B569" s="1" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="570" spans="1:2">
       <c r="A570" t="s">
         <v>595</v>
       </c>
-    </row>
-    <row r="571" spans="1:1">
+      <c r="B570" s="1" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="571" spans="1:2">
       <c r="A571" t="s">
         <v>457</v>
       </c>
-    </row>
-    <row r="572" spans="1:1">
+      <c r="B571" s="1" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="572" spans="1:2">
       <c r="A572" t="s">
         <v>596</v>
       </c>
-    </row>
-    <row r="573" spans="1:1">
+      <c r="B572" s="1" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="573" spans="1:2">
       <c r="A573" t="s">
         <v>458</v>
       </c>
-    </row>
-    <row r="574" spans="1:1">
+      <c r="B573" s="1" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="574" spans="1:2">
       <c r="A574" t="s">
         <v>606</v>
       </c>
-    </row>
-    <row r="575" spans="1:1">
+      <c r="B574" s="1" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="575" spans="1:2">
       <c r="A575" t="s">
         <v>459</v>
       </c>
-    </row>
-    <row r="576" spans="1:1">
+      <c r="B575" s="1" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="576" spans="1:2">
       <c r="A576" t="s">
         <v>460</v>
       </c>
-    </row>
-    <row r="577" spans="1:1">
+      <c r="B576" s="1" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="577" spans="1:2">
       <c r="A577" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="578" spans="1:1">
+      <c r="B577" s="1" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="578" spans="1:2">
       <c r="A578" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="579" spans="1:1">
+      <c r="B578" s="1" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="579" spans="1:2">
       <c r="A579" t="s">
         <v>463</v>
       </c>
-    </row>
-    <row r="580" spans="1:1">
+      <c r="B579" s="1" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="580" spans="1:2">
       <c r="A580" t="s">
         <v>464</v>
       </c>
-    </row>
-    <row r="581" spans="1:1">
+      <c r="B580" s="1" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="581" spans="1:2">
       <c r="A581" t="s">
         <v>465</v>
       </c>
-    </row>
-    <row r="582" spans="1:1">
+      <c r="B581" s="1" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="582" spans="1:2">
       <c r="A582" t="s">
         <v>466</v>
       </c>
-    </row>
-    <row r="583" spans="1:1">
+      <c r="B582" s="1" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="583" spans="1:2">
       <c r="A583" t="s">
         <v>467</v>
       </c>
-    </row>
-    <row r="584" spans="1:1">
+      <c r="B583" s="1" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="584" spans="1:2">
       <c r="A584" t="s">
         <v>468</v>
       </c>
-    </row>
-    <row r="585" spans="1:1">
+      <c r="B584" s="1" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="585" spans="1:2">
       <c r="A585" t="s">
         <v>469</v>
       </c>
-    </row>
-    <row r="586" spans="1:1">
+      <c r="B585" s="1" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="586" spans="1:2">
       <c r="A586" t="s">
         <v>470</v>
       </c>
-    </row>
-    <row r="587" spans="1:1">
+      <c r="B586" s="1" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="587" spans="1:2">
       <c r="A587" t="s">
         <v>471</v>
       </c>
-    </row>
-    <row r="588" spans="1:1">
+      <c r="B587" s="1" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="588" spans="1:2">
       <c r="A588" t="s">
         <v>472</v>
       </c>
-    </row>
-    <row r="589" spans="1:1">
+      <c r="B588" s="1" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="589" spans="1:2">
       <c r="A589" t="s">
         <v>473</v>
       </c>
-    </row>
-    <row r="590" spans="1:1">
+      <c r="B589" s="1" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="590" spans="1:2">
       <c r="A590" t="s">
         <v>474</v>
       </c>
-    </row>
-    <row r="591" spans="1:1">
+      <c r="B590" s="1" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="591" spans="1:2">
       <c r="A591" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="592" spans="1:1">
+      <c r="B591" s="1" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="592" spans="1:2">
       <c r="A592" t="s">
         <v>476</v>
       </c>
-    </row>
-    <row r="593" spans="1:1">
+      <c r="B592" s="1" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="593" spans="1:2">
       <c r="A593" t="s">
         <v>477</v>
       </c>
-    </row>
-    <row r="594" spans="1:1">
+      <c r="B593" s="1" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="594" spans="1:2">
       <c r="A594" t="s">
         <v>478</v>
       </c>
-    </row>
-    <row r="595" spans="1:1">
+      <c r="B594" s="1" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="595" spans="1:2">
       <c r="A595" t="s">
         <v>479</v>
       </c>
-    </row>
-    <row r="596" spans="1:1">
+      <c r="B595" s="1" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="596" spans="1:2">
       <c r="A596" t="s">
         <v>480</v>
       </c>
-    </row>
-    <row r="597" spans="1:1">
+      <c r="B596" s="1" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="597" spans="1:2">
       <c r="A597" t="s">
         <v>597</v>
       </c>
-    </row>
-    <row r="598" spans="1:1">
+      <c r="B597" s="1" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="598" spans="1:2">
       <c r="A598" t="s">
         <v>481</v>
       </c>
-    </row>
-    <row r="599" spans="1:1">
+      <c r="B598" s="1" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="599" spans="1:2">
       <c r="A599" t="s">
         <v>482</v>
       </c>
-    </row>
-    <row r="600" spans="1:1">
+      <c r="B599" s="1" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="600" spans="1:2">
       <c r="A600" t="s">
         <v>483</v>
       </c>
-    </row>
-    <row r="601" spans="1:1">
+      <c r="B600" s="1" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="601" spans="1:2">
       <c r="A601" t="s">
         <v>484</v>
       </c>
-    </row>
-    <row r="602" spans="1:1">
+      <c r="B601" s="1" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="602" spans="1:2">
       <c r="A602" t="s">
         <v>598</v>
       </c>
-    </row>
-    <row r="603" spans="1:1">
+      <c r="B602" s="1" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="603" spans="1:2">
       <c r="A603" t="s">
         <v>485</v>
       </c>
-    </row>
-    <row r="604" spans="1:1">
+      <c r="B603" s="1" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="604" spans="1:2">
       <c r="A604" t="s">
         <v>486</v>
       </c>
-    </row>
-    <row r="605" spans="1:1">
+      <c r="B604" s="1" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="605" spans="1:2">
       <c r="A605" t="s">
         <v>487</v>
       </c>
-    </row>
-    <row r="606" spans="1:1">
+      <c r="B605" s="1" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="606" spans="1:2">
       <c r="A606" t="s">
         <v>599</v>
       </c>
-    </row>
-    <row r="607" spans="1:1">
+      <c r="B606" s="1" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="607" spans="1:2">
       <c r="A607" t="s">
         <v>488</v>
       </c>
-    </row>
-    <row r="608" spans="1:1">
+      <c r="B607" s="1" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="608" spans="1:2">
       <c r="A608" t="s">
         <v>489</v>
       </c>
-    </row>
-    <row r="609" spans="1:1">
+      <c r="B608" s="1" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="609" spans="1:2">
       <c r="A609" t="s">
         <v>490</v>
       </c>
-    </row>
-    <row r="610" spans="1:1">
+      <c r="B609" s="1" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="610" spans="1:2">
       <c r="A610" t="s">
         <v>600</v>
       </c>
-    </row>
-    <row r="611" spans="1:1">
+      <c r="B610" s="1" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="611" spans="1:2">
       <c r="A611" t="s">
         <v>491</v>
       </c>
-    </row>
-    <row r="612" spans="1:1">
+      <c r="B611" s="1" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="612" spans="1:2">
       <c r="A612" t="s">
         <v>492</v>
       </c>
-    </row>
-    <row r="613" spans="1:1">
+      <c r="B612" s="1" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="613" spans="1:2">
       <c r="A613" t="s">
         <v>493</v>
       </c>
-    </row>
-    <row r="614" spans="1:1">
+      <c r="B613" s="1" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="614" spans="1:2">
       <c r="A614" t="s">
         <v>494</v>
       </c>
-    </row>
-    <row r="615" spans="1:1">
+      <c r="B614" s="1" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="615" spans="1:2">
       <c r="A615" t="s">
         <v>495</v>
       </c>
-    </row>
-    <row r="616" spans="1:1">
+      <c r="B615" s="1" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="616" spans="1:2">
       <c r="A616" t="s">
         <v>496</v>
       </c>
-    </row>
-    <row r="617" spans="1:1">
+      <c r="B616" s="1" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="617" spans="1:2">
       <c r="A617" t="s">
         <v>497</v>
       </c>
-    </row>
-    <row r="618" spans="1:1">
+      <c r="B617" s="1" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="618" spans="1:2">
       <c r="A618" t="s">
         <v>498</v>
       </c>
-    </row>
-    <row r="619" spans="1:1">
+      <c r="B618" s="1" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="619" spans="1:2">
       <c r="A619" t="s">
         <v>601</v>
       </c>
-    </row>
-    <row r="620" spans="1:1">
+      <c r="B619" s="1" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="620" spans="1:2">
       <c r="A620" t="s">
         <v>499</v>
       </c>
-    </row>
-    <row r="621" spans="1:1">
+      <c r="B620" s="1" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="621" spans="1:2">
       <c r="A621" t="s">
         <v>489</v>
       </c>
+      <c r="B621" s="1" t="s">
+        <v>603</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B13 A1:A1048576">
-    <cfRule type="containsText" dxfId="16" priority="8" operator="containsText" text="\darkradiant">
+    <cfRule type="containsText" dxfId="28" priority="8" operator="containsText" text="\darkradiant">
       <formula>NOT(ISERROR(SEARCH("\darkradiant",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B621">
-    <cfRule type="notContainsText" dxfId="15" priority="5" operator="notContains" text="ok">
+    <cfRule type="notContainsText" dxfId="27" priority="5" operator="notContains" text="ok">
       <formula>ISERROR(SEARCH("ok",B2))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="7" operator="containsText" text="ok">
+    <cfRule type="containsText" dxfId="26" priority="7" operator="containsText" text="ok">
       <formula>NOT(ISERROR(SEARCH("ok",B2)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>